<commit_message>
much happier with structure now. Add Employee reimplemented
</commit_message>
<xml_diff>
--- a/UML.xlsx
+++ b/UML.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\git_repos\ShopSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D6B167-8FAD-4FE2-9246-D207460E865C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57E4319-C721-4421-B979-8B872D32B264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MVC Structure" sheetId="1" r:id="rId1"/>
+    <sheet name="Model" sheetId="2" r:id="rId2"/>
+    <sheet name="View" sheetId="3" r:id="rId3"/>
+    <sheet name="Controller" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,14 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
   <si>
     <t>View</t>
   </si>
   <si>
-    <t xml:space="preserve"> - </t>
-  </si>
-  <si>
     <t>DatabaseAccessObject</t>
   </si>
   <si>
@@ -112,9 +112,6 @@
     <t>ViewSplash()</t>
   </si>
   <si>
-    <t xml:space="preserve"> - viewHumanResourcesController : ViewHumanResourcesController</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - employeeDetailAdd : ViewEmployeeDetail</t>
   </si>
   <si>
@@ -157,20 +154,170 @@
     <t>ViewEmployeeDetailControllerEdit</t>
   </si>
   <si>
-    <t xml:space="preserve"> - validateEmployeeDataFromGUI() : boolean[]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + addEmployeeToDatabase() : void</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - colorBorders(boolean[]) : void</t>
+    <t xml:space="preserve"> + DataBaseAccessObject(String)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - testConnection(String) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - getConnection() : Connection</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + getEmployees() : ArrayList&lt;Employee&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + addEmployee(Employee) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - addPerson(Person) : int</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - closeQuietly(AutoCloseable) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - viewHumanResourcesController : hrController</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + ViewHumanResources()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + refresh() : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + getEmployeeDetailAdd() : ViewEmployeeDetail</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - setEmployeeDetailAdd() : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + getEmployeeDetailEdit() : ViewEmployeeDetail</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - setEmployeeDetailEdit() : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + main(String[]) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + addEmployeeToDatabase(Employee) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + showEmployeeDetailAdd() : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + showHumanResources() : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + getEmployeesFromDatabase() : ArrayList&lt;Employee&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + employeeToDatabase() : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + clearFields() : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - colorBordersBlack() : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + getForename() : String</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + getSurname() : String</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + getEmail() : String</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + getPhoneNumber() : String</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + getHourlyRate() : String</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + getWeeklyHours() : String</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + getStartDate() : LocalDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + getEndDate() : LocalDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - validationErrorString : String</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - model : HumanResourcesModel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - formatter : DateTimeFormatter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> # getAndClearValidationMessage() : String</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ colorBorders(boolean[]) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ setForenameTextField(String) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ getForenameTextField() : TextField</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ setSurnameTextField(String) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ getSurnameTextField() : TextField</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ setEmailTextField(String) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ getEmailTextField() : TextField</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ setPhoneNumberTextField(String) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ getPhoneNumberTextField() : TextField</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ setHourlyRateTextField(String) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ getHourlyRateTextField() : TextField</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ setWeeklyHoursTextField(String) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ getWeeklyHoursTextField() : TextField</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ setStartDateDatePicker(LocalDate) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ getStartDateDatePicker() : DatePicker</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ setEndDateDatePicker(LocalDate) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ getEndDateDatePicker() : DatePicker</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> # validateEmployeeDataFromGUI() : boolean[]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + FIELDS_TO_VALIDATE : int</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +333,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -195,7 +350,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -212,18 +367,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -245,6 +436,119 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FAAA0E3-1AA2-4286-AC58-9DD6E543066A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1428750" y="4848225"/>
+          <a:ext cx="2800350" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1019175</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C8710FA-5333-46E9-8B14-9478A1905377}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5305425" y="5038725"/>
+          <a:ext cx="3733800" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -258,10 +562,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{591F4875-8193-4EF9-8524-118BBC5612DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D435EA10-627B-4EBA-A2CA-77B3F9BC5598}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -269,8 +573,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9858375" y="304800"/>
-          <a:ext cx="1057275" cy="9525"/>
+          <a:off x="3743325" y="304800"/>
+          <a:ext cx="542925" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -311,10 +615,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82B7DA21-06A5-4290-9218-7ED960CC20AB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36FFB406-43FB-4FF8-BFB6-2BBFC162335F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -322,8 +626,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="9877425" y="457200"/>
-          <a:ext cx="1085850" cy="1209675"/>
+          <a:off x="3762375" y="457200"/>
+          <a:ext cx="523875" cy="1209675"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -351,92 +655,37 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FAAA0E3-1AA2-4286-AC58-9DD6E543066A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7776450-6ADE-4857-A7D9-B612A6B1B93E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="1600200"/>
-          <a:ext cx="476250" cy="9525"/>
+        <a:xfrm flipH="1">
+          <a:off x="10877550" y="1628775"/>
+          <a:ext cx="533400" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
-          <a:headEnd type="triangle"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C8710FA-5333-46E9-8B14-9478A1905377}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3914775" y="1809750"/>
-          <a:ext cx="457200" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="triangle"/>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -723,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G29"/>
+  <dimension ref="A2:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,183 +987,84 @@
     <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E29" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -922,4 +1072,363 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{074D839C-748A-4B26-A962-8D9EEC66B1DB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B264D077-796C-4049-9AF2-7292CF53A09B}">
+  <dimension ref="A2:G49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E45" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E46" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E47" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E48" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1866C118-A270-4E41-9562-411F5590B1C9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding in javadoc and fixing a few minor bugs
</commit_message>
<xml_diff>
--- a/UML.xlsx
+++ b/UML.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\git_repos\ShopSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57E4319-C721-4421-B979-8B872D32B264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1F72AE-B8A0-4794-8314-A589074DE67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MVC Structure" sheetId="1" r:id="rId1"/>
@@ -317,7 +317,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,6 +330,13 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -394,10 +404,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -406,17 +417,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,13 +565,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -572,12 +585,14 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="3743325" y="304800"/>
-          <a:ext cx="542925" cy="9525"/>
+        <a:xfrm rot="10800000">
+          <a:off x="3743325" y="314326"/>
+          <a:ext cx="495300" cy="161925"/>
         </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -1923"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -603,68 +618,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36FFB406-43FB-4FF8-BFB6-2BBFC162335F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="3762375" y="457200"/>
-          <a:ext cx="523875" cy="1209675"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -678,12 +640,235 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="10877550" y="1628775"/>
-          <a:ext cx="533400" cy="0"/>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="2557463" y="6396038"/>
+          <a:ext cx="2809875" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 99831"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38103</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>200026</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3A70C21-5834-4DC6-9429-AF80EF324309}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3714753" y="190503"/>
+          <a:ext cx="4467223" cy="1647823"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 107"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11" descr="uses">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1875563-0960-4CBB-BA25-965F9D8BED81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7477125" y="2000250"/>
+          <a:ext cx="428625" cy="142875"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{912D3250-B75A-41CA-9D97-D92844A9FC58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7724775" y="1171575"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9527</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{141FAB26-0CEA-4B6D-A203-B0000FD842DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="3248026" y="847726"/>
+          <a:ext cx="1409698" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100000"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -975,7 +1160,7 @@
   <dimension ref="A2:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,12 +1173,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
@@ -1007,7 +1192,7 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="14" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1088,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B264D077-796C-4049-9AF2-7292CF53A09B}">
-  <dimension ref="A2:G49"/>
+  <dimension ref="A2:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,315 +1287,337 @@
     <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="G7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E14" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="5" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="6" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="11" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="7" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="8" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="8" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="8" t="s">
+      <c r="C41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="8" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="8" t="s">
+      <c r="C43" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="8" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E27" s="8" t="s">
+      <c r="C45" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E28" s="8" t="s">
+      <c r="C46" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E29" s="8" t="s">
+      <c r="C47" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E30" s="8" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E31" s="8" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E32" s="8" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" s="8" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" s="8" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35" s="8" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E36" s="8" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E37" s="8" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E38" s="8" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E39" s="8" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E40" s="8" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E41" s="8" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E42" s="8" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E43" s="8" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E44" s="8" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E45" s="8" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E46" s="8" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E47" s="8" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E48" s="8" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E49" s="8" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>